<commit_message>
update: changed title and favicon and changes sample question
</commit_message>
<xml_diff>
--- a/frontend/public/questions_template.xlsx
+++ b/frontend/public/questions_template.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>title</t>
   </si>
@@ -37,31 +37,34 @@
     <t>tags</t>
   </si>
   <si>
-    <t>Which formula represents the Pythagorean theorem?</t>
-  </si>
-  <si>
-    <t>Select the correct expression</t>
-  </si>
-  <si>
-    <t>Class 10</t>
+    <t>Which HTTP status code means "Not Found"?</t>
+  </si>
+  <si>
+    <t>Select the correct numeric status code</t>
+  </si>
+  <si>
+    <t>Web Dev</t>
   </si>
   <si>
     <t>single_choice</t>
   </si>
   <si>
-    <t>["a^2 + b^2 = c^2","a^2 = b^2 + c^2","a + b = c"]</t>
-  </si>
-  <si>
-    <t>["a^2 + b^2 = c^2"]</t>
-  </si>
-  <si>
-    <t>geometry,power</t>
-  </si>
-  <si>
-    <t>Explain the Pythagorean theorem</t>
-  </si>
-  <si>
-    <t>Open-ended explanation</t>
+    <t>["200","301","404"]</t>
+  </si>
+  <si>
+    <t>["404"]</t>
+  </si>
+  <si>
+    <t>http,status</t>
+  </si>
+  <si>
+    <t>Explain the difference between React useState and useEffect</t>
+  </si>
+  <si>
+    <t>Provide a short comparison of the two hooks</t>
+  </si>
+  <si>
+    <t>Frontend</t>
   </si>
   <si>
     <t>text</t>
@@ -70,28 +73,28 @@
     <t/>
   </si>
   <si>
-    <t>geometry</t>
-  </si>
-  <si>
-    <t>Select all prime numbers</t>
-  </si>
-  <si>
-    <t>Choose numbers that are prime</t>
-  </si>
-  <si>
-    <t>Class 8</t>
+    <t>react,hooks</t>
+  </si>
+  <si>
+    <t>Which of the following are fruits?</t>
+  </si>
+  <si>
+    <t>Select all that are fruits</t>
+  </si>
+  <si>
+    <t>General Knowledge</t>
   </si>
   <si>
     <t>multi_choice</t>
   </si>
   <si>
-    <t>["2","3","4","5"]</t>
-  </si>
-  <si>
-    <t>["2","3","5"]</t>
-  </si>
-  <si>
-    <t>math,number</t>
+    <t>["Apple","Carrot","Banana","Potato"]</t>
+  </si>
+  <si>
+    <t>["Apple","Banana"]</t>
+  </si>
+  <si>
+    <t>food,fruit</t>
   </si>
 </sst>
 </file>
@@ -531,48 +534,48 @@
         <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G3">
         <v>5</v>
       </c>
       <c r="H3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G4">
         <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>